<commit_message>
No need for cost helper. There were label 'bugs' in the replace_effect_codes function. The prices should be labelled because the sub_codes needs these ref values in the multiplication. It would make the replace_effect_codes function sleeker, if we'd label the rest only after... But anyways, it should do the trick now!
</commit_message>
<xml_diff>
--- a/data-raw/labels_de.xlsx
+++ b/data-raw/labels_de.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vehicle_type" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="69">
   <si>
     <t xml:space="preserve">from</t>
   </si>
@@ -172,19 +172,10 @@
     <t xml:space="preserve">revert</t>
   </si>
   <si>
-    <t xml:space="preserve">Gasoline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electric</t>
+    <t xml:space="preserve">Elektrisch</t>
   </si>
   <si>
     <t xml:space="preserve">Hybrid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plug-in hybrid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elektrisch</t>
   </si>
   <si>
     <t xml:space="preserve">Plug-in Hybrid</t>
@@ -360,7 +351,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
   </cols>
@@ -501,7 +492,7 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -521,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -529,7 +520,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -554,7 +545,7 @@
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -574,7 +565,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -582,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -607,7 +598,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -627,7 +618,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,7 +626,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +651,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -670,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,7 +677,7 @@
         <v>0.7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -697,7 +688,7 @@
         <v>1.3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -722,7 +713,7 @@
       <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
   </cols>
@@ -745,7 +736,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -753,7 +744,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,7 +752,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -786,7 +777,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -806,7 +797,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -814,7 +805,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -839,7 +830,7 @@
       <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -859,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -867,7 +858,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -892,7 +883,7 @@
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -912,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -942,7 +933,7 @@
       <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -952,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,7 +959,7 @@
         <v>0.7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,7 +970,7 @@
         <v>1.3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1004,7 +995,7 @@
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1014,7 +1005,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,7 +1021,7 @@
         <v>0.7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,7 +1032,7 @@
         <v>1.3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1066,7 +1057,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.92"/>
   </cols>
@@ -1157,281 +1148,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C23"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="23.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1442,7 +1158,11 @@
       <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="23.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.16"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1468,7 +1188,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>36</v>
@@ -1479,7 +1199,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>36</v>
@@ -1489,8 +1209,8 @@
       <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>45</v>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>36</v>
@@ -1501,7 +1221,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>36</v>
@@ -1512,7 +1232,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>36</v>
@@ -1531,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>41</v>
@@ -1542,7 +1262,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>41</v>
@@ -1553,7 +1273,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>41</v>
@@ -1564,7 +1284,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>41</v>
@@ -1575,6 +1295,277 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="0" t="s">
@@ -1605,7 +1596,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>26</v>
@@ -1616,7 +1607,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>28</v>
@@ -1627,7 +1618,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>31</v>
@@ -1663,7 +1654,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>43</v>
@@ -1674,7 +1665,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>43</v>
@@ -1685,7 +1676,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>43</v>
@@ -1713,7 +1704,7 @@
       <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1723,7 +1714,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1739,7 +1730,7 @@
         <v>0.7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,7 +1741,7 @@
         <v>1.3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1775,7 +1766,7 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1785,7 +1776,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,7 +1792,7 @@
         <v>0.7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,7 +1803,7 @@
         <v>1.3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1837,7 +1828,7 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1847,7 +1838,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,7 +1854,7 @@
         <v>0.7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1874,7 +1865,7 @@
         <v>1.3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1899,7 +1890,7 @@
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1919,7 +1910,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,7 +1918,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1952,7 +1943,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1972,7 +1963,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,7 +1971,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Modular Travel Card to Regional Season Ticket and 1-2 zones to 2 zones.
</commit_message>
<xml_diff>
--- a/data-raw/labels_de.xlsx
+++ b/data-raw/labels_de.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="vehicle_type" sheetId="1" state="visible" r:id="rId2"/>
@@ -229,7 +229,7 @@
     <t xml:space="preserve">Halbtax</t>
   </si>
   <si>
-    <t xml:space="preserve">Modul-Abo (Verbund)</t>
+    <t xml:space="preserve">Regionales Saison-Abonnement</t>
   </si>
   <si>
     <t xml:space="preserve">Erste</t>
@@ -238,7 +238,7 @@
     <t xml:space="preserve">Zweite</t>
   </si>
   <si>
-    <t xml:space="preserve">1-2 Zonen</t>
+    <t xml:space="preserve">2 Zonen</t>
   </si>
   <si>
     <t xml:space="preserve">Ganzer Tarifverbund</t>
@@ -351,7 +351,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
   </cols>
@@ -492,7 +492,7 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -545,7 +545,7 @@
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -598,7 +598,7 @@
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -651,7 +651,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -710,10 +710,10 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
   </cols>
@@ -777,7 +777,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -826,11 +826,11 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -883,7 +883,7 @@
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -933,7 +933,7 @@
       <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -995,7 +995,7 @@
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1057,7 +1057,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.92"/>
   </cols>
@@ -1158,7 +1158,7 @@
       <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.16"/>
@@ -1429,11 +1429,11 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1704,7 +1704,7 @@
       <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1766,7 +1766,7 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1828,7 +1828,7 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1890,7 +1890,7 @@
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1943,7 +1943,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>